<commit_message>
Important commit: add Sedimentary
Add Sediment data into data assessment workflow
Data_assesment_writetxt.R is now writing in Rich Text File to get Word
formatting (bold, italic, …)
Add Maps
Add station description
</commit_message>
<xml_diff>
--- a/LC Description/LoadCell_details.xlsx
+++ b/LC Description/LoadCell_details.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-25540" yWindow="440" windowWidth="24860" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="-25540" yWindow="440" windowWidth="24860" windowHeight="17060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="LoadCell_details_coord_UTM33.tx" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="64">
   <si>
     <t>ObjectID</t>
   </si>
@@ -187,9 +187,6 @@
   </si>
   <si>
     <t>2008.06.19</t>
-  </si>
-  <si>
-    <t>2001.20.03</t>
   </si>
   <si>
     <t>2003.11.11</t>
@@ -221,9 +218,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="168" formatCode="0.0"/>
-    <numFmt numFmtId="171" formatCode="0.00000000000"/>
-    <numFmt numFmtId="179" formatCode="0.000000E+00;\_x0000_"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.00000000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000E+00;\_x0000_"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -278,8 +275,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="119">
+  <cellStyleXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -404,16 +415,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="119">
+  <cellStyles count="133">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -473,6 +484,13 @@
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -532,6 +550,13 @@
     <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -864,7 +889,9 @@
   <dimension ref="A1:AE10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <pane xSplit="2940" activePane="topRight"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection pane="topRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1149,16 +1176,17 @@
         <v>6</v>
       </c>
       <c r="AA3">
-        <v>384430.16310499999</v>
+        <v>446820</v>
       </c>
       <c r="AB3">
-        <v>6420486.1012599999</v>
+        <v>7395454</v>
       </c>
       <c r="AC3" t="s">
         <v>28</v>
       </c>
-      <c r="AD3" s="3" t="s">
-        <v>28</v>
+      <c r="AD3" s="3">
+        <f>SQRT((AA3-$AA$7)^2+(AB3-$AB$7)^2)</f>
+        <v>20.617851356242952</v>
       </c>
       <c r="AE3" s="5" t="s">
         <v>28</v>
@@ -1184,7 +1212,7 @@
         <v>52</v>
       </c>
       <c r="G4" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="H4">
         <v>34892</v>
@@ -1250,11 +1278,11 @@
         <v>632.59</v>
       </c>
       <c r="AD4" s="3">
-        <f>SQRT((AA4-$AA$7)^2+(AB4-$AB$7)^2)</f>
+        <f t="shared" ref="AD4:AD10" si="0">SQRT((AA4-$AA$7)^2+(AB4-$AB$7)^2)</f>
         <v>7.1656626087962287</v>
       </c>
       <c r="AE4" s="5">
-        <f>AC4-$AC$7</f>
+        <f t="shared" ref="AE4:AE10" si="1">AC4-$AC$7</f>
         <v>1.9800000000000182</v>
       </c>
     </row>
@@ -1344,11 +1372,11 @@
         <v>632.53</v>
       </c>
       <c r="AD5" s="3">
-        <f>SQRT((AA5-$AA$7)^2+(AB5-$AB$7)^2)</f>
+        <f t="shared" si="0"/>
         <v>10.115102343677496</v>
       </c>
       <c r="AE5" s="5">
-        <f>AC5-$AC$7</f>
+        <f t="shared" si="1"/>
         <v>1.9199999999999591</v>
       </c>
     </row>
@@ -1438,11 +1466,11 @@
         <v>631.73</v>
       </c>
       <c r="AD6" s="3">
-        <f>SQRT((AA6-$AA$7)^2+(AB6-$AB$7)^2)</f>
+        <f t="shared" si="0"/>
         <v>0.43783775702434735</v>
       </c>
       <c r="AE6" s="5">
-        <f>AC6-$AC$7</f>
+        <f t="shared" si="1"/>
         <v>1.1200000000000045</v>
       </c>
     </row>
@@ -1532,11 +1560,11 @@
         <v>630.61</v>
       </c>
       <c r="AD7" s="3">
-        <f>SQRT((AA7-$AA$7)^2+(AB7-$AB$7)^2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AE7" s="5">
-        <f>AC7-$AC$7</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1560,7 +1588,7 @@
         <v>52</v>
       </c>
       <c r="G8" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H8">
         <v>36992</v>
@@ -1578,10 +1606,10 @@
         <v>1.7080800000000001E-5</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O8" t="s">
         <v>55</v>
@@ -1629,11 +1657,11 @@
         <v>630.85</v>
       </c>
       <c r="AD8" s="3">
-        <f>SQRT((AA8-$AA$7)^2+(AB8-$AB$7)^2)</f>
+        <f t="shared" si="0"/>
         <v>13.579094201268907</v>
       </c>
       <c r="AE8" s="5">
-        <f>AC8-$AC$7</f>
+        <f t="shared" si="1"/>
         <v>0.24000000000000909</v>
       </c>
     </row>
@@ -1657,7 +1685,7 @@
         <v>53</v>
       </c>
       <c r="G9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H9">
         <v>37692</v>
@@ -1678,7 +1706,7 @@
         <v>46</v>
       </c>
       <c r="N9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O9" t="s">
         <v>28</v>
@@ -1702,7 +1730,7 @@
         <v>1.641125E-5</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W9" t="s">
         <v>5</v>
@@ -1726,11 +1754,11 @@
         <v>630.70000000000005</v>
       </c>
       <c r="AD9" s="3">
-        <f>SQRT((AA9-$AA$7)^2+(AB9-$AB$7)^2)</f>
+        <f t="shared" si="0"/>
         <v>21.332935673817211</v>
       </c>
       <c r="AE9" s="5">
-        <f>AC9-$AC$7</f>
+        <f t="shared" si="1"/>
         <v>9.0000000000031832E-2</v>
       </c>
     </row>
@@ -1754,7 +1782,7 @@
         <v>53</v>
       </c>
       <c r="G10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H10">
         <v>38292</v>
@@ -1772,10 +1800,10 @@
         <v>1.6882189999999998E-5</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O10" t="s">
         <v>28</v>
@@ -1799,7 +1827,7 @@
         <v>1.5352449999999999E-5</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W10" t="s">
         <v>5</v>
@@ -1823,11 +1851,11 @@
         <v>630.6</v>
       </c>
       <c r="AD10" s="3">
-        <f>SQRT((AA10-$AA$7)^2+(AB10-$AB$7)^2)</f>
+        <f t="shared" si="0"/>
         <v>21.080406987502489</v>
       </c>
       <c r="AE10" s="5">
-        <f>AC10-$AC$7</f>
+        <f t="shared" si="1"/>
         <v>-9.9999999999909051E-3</v>
       </c>
     </row>

</xml_diff>